<commit_message>
add drafts, regional draft and data updates
</commit_message>
<xml_diff>
--- a/data/regional_profile_raceovertime.xlsx
+++ b/data/regional_profile_raceovertime.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11027"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/henrydemarco/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://myuva-my.sharepoint.com/personal/eam5hc_virginia_edu/Documents/projects/regional-equity-profile/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3861BBE3-5794-174D-8EDB-8127956384EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="16540" windowHeight="16480" firstSheet="1" activeTab="1" xr2:uid="{8021F1F0-A3AD-1141-A51F-B071934EF0DC}"/>
+    <workbookView xWindow="41940" yWindow="1640" windowWidth="24520" windowHeight="16980" firstSheet="1" activeTab="2" xr2:uid="{8021F1F0-A3AD-1141-A51F-B071934EF0DC}"/>
   </bookViews>
   <sheets>
     <sheet name="social_exp_charlottesville" sheetId="1" r:id="rId1"/>
@@ -1901,7 +1901,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2024D05D-E961-A644-95D0-D9577C4FEBFA}">
   <dimension ref="A1:R56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
@@ -2757,8 +2757,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59BC323E-7B1A-874F-8A4A-87D54C2905E2}">
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
update data/added ACS 2023 data
</commit_message>
<xml_diff>
--- a/data/regional_profile_raceovertime.xlsx
+++ b/data/regional_profile_raceovertime.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11027"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://myuva-my.sharepoint.com/personal/eam5hc_virginia_edu/Documents/projects/regional-equity-profile/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3861BBE3-5794-174D-8EDB-8127956384EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{3861BBE3-5794-174D-8EDB-8127956384EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{41EDA370-52B4-3643-8148-45483E180AF3}"/>
   <bookViews>
-    <workbookView xWindow="41940" yWindow="1640" windowWidth="24520" windowHeight="16980" firstSheet="1" activeTab="2" xr2:uid="{8021F1F0-A3AD-1141-A51F-B071934EF0DC}"/>
+    <workbookView xWindow="8700" yWindow="760" windowWidth="25860" windowHeight="16740" activeTab="4" xr2:uid="{8021F1F0-A3AD-1141-A51F-B071934EF0DC}"/>
   </bookViews>
   <sheets>
     <sheet name="social_exp_charlottesville" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="69">
   <si>
     <t>Total Population:</t>
   </si>
@@ -245,6 +245,9 @@
   </si>
   <si>
     <t>nonwhite_per</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -689,7 +692,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9563645-D09E-9746-AFC1-7DA7C08A9EC2}">
   <dimension ref="A1:L142"/>
   <sheetViews>
-    <sheetView topLeftCell="A51" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D80" sqref="D80"/>
     </sheetView>
   </sheetViews>
@@ -2757,7 +2760,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59BC323E-7B1A-874F-8A4A-87D54C2905E2}">
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
@@ -3503,8 +3506,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A30F7007-796F-6949-89DC-83451E132588}">
   <dimension ref="A1:D155"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3515,6 +3518,9 @@
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1">
         <v>1790</v>
+      </c>
+      <c r="B1" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>